<commit_message>
Dataframes pass by reference when you create a DF from another DF.... I hate python
</commit_message>
<xml_diff>
--- a/Schedules/CM_course_schedule.xlsx
+++ b/Schedules/CM_course_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>TIME</t>
   </si>
@@ -62,12 +62,10 @@
   </si>
   <si>
     <t>3
-AV-410-03809-Balch-EAX-011
 CM-200-03811-Mohamed Ali-IDE-318</t>
   </si>
   <si>
     <t>5
-AM-201-05816-Balch-EAX-011
 CM-320-05815-nan-EAX-015
 CM-320-05815-nan-EAX-016</t>
   </si>
@@ -76,7 +74,6 @@
   </si>
   <si>
     <t>9
-AM-220-09801-Wyman-EAX-009
 CSM-305-09814-nan-EAX-015
 CSM-305-09814-nan-EAX-016</t>
   </si>
@@ -98,19 +95,16 @@
   </si>
   <si>
     <t>4
-AV-306-04805-Breuder-EAX-009
 CM-375-04808-Regnery-EAX-017</t>
   </si>
   <si>
     <t>13
-AV-300-13804-Wyman-EAX-010
 CSM-225-13810-Trottier-EAX-017
 CSM-199-13805-nan-EAX-015
 CSM-199-13805-nan-EAX-016</t>
   </si>
   <si>
-    <t>14
-AT-410-14801-Wyman-EAX-012</t>
+    <t>14</t>
   </si>
   <si>
     <t>10</t>
@@ -120,7 +114,6 @@
   </si>
   <si>
     <t>21
-AM-340-21802-Moon-IDE-317
 CSM-300-21804-Michienzi-EAX-015
 CSM-300-21804-Michienzi-EAX-016
 CM-415-21803-Rounds-IDE-318</t>
@@ -135,12 +128,10 @@
     <t>6</t>
   </si>
   <si>
-    <t>8
-AV-205-08815-LaFauci-IDE-209</t>
-  </si>
-  <si>
-    <t>12
-AM-340L-12802-Moon-IDE-317</t>
+    <t>8</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>20
@@ -149,20 +140,10 @@
 CSM-220-20806-Michienzi-EAX-016</t>
   </si>
   <si>
-    <t>13
-AV-300-13804-Wyman-EAX-010</t>
-  </si>
-  <si>
-    <t>5
-AM-201-05816-Balch-EAX-011
-AT-410L-05804-Adelizzi-EAX-022
-AT-410L-05804-Adelizzi-EAX-023
-CM-320-05815-nan-EAX-015
-CM-320-05815-nan-EAX-016</t>
-  </si>
-  <si>
-    <t>9
-AM-220-09801-Wyman-EAX-009</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>11
@@ -171,7 +152,6 @@
   </si>
   <si>
     <t>21
-AM-340-21802-Moon-IDE-317
 CM-415-21803-Rounds-IDE-318</t>
   </si>
   <si>
@@ -179,15 +159,13 @@
   </si>
   <si>
     <t>4.0
-AV-306-04805-Breuder-EAX-009
 CM-375-04808-Regnery-EAX-017</t>
   </si>
   <si>
     <t>6.0</t>
   </si>
   <si>
-    <t>8.0
-AV-205-08815-LaFauci-IDE-209</t>
+    <t>8.0</t>
   </si>
   <si>
     <t>10.0</t>
@@ -597,7 +575,7 @@
         <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -617,7 +595,7 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -634,10 +612,10 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -657,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -674,10 +652,10 @@
         <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -694,10 +672,10 @@
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -714,10 +692,10 @@
         <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -737,7 +715,7 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -757,7 +735,7 @@
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TBD instead of nan for classes undetermined
</commit_message>
<xml_diff>
--- a/Schedules/CM_course_schedule.xlsx
+++ b/Schedules/CM_course_schedule.xlsx
@@ -79,8 +79,8 @@
   </si>
   <si>
     <t>11
-CSM-305-09814-nan-EAX-015
-CSM-305-09814-nan-EAX-016</t>
+CSM-305-09814-TBD-EAX-015
+CSM-305-09814-TBD-EAX-016</t>
   </si>
   <si>
     <t>20
@@ -108,8 +108,8 @@
   <si>
     <t>14
 CSM-225-13810-Trottier-EAX-017
-CSM-199-13805-nan-EAX-015
-CSM-199-13805-nan-EAX-016</t>
+CSM-199-13805-TBD-EAX-015
+CSM-199-13805-TBD-EAX-016</t>
   </si>
   <si>
     <t>10</t>
@@ -168,8 +168,8 @@
   <si>
     <t>21
 CM-415-21803-Rounds-IDE-318
-CSM-199-11810-nan-EAX-015
-CSM-199-11810-nan-EAX-016</t>
+CSM-199-11810-TBD-EAX-015
+CSM-199-11810-TBD-EAX-016</t>
   </si>
   <si>
     <t>23</t>

</xml_diff>

<commit_message>
Fixed TBD issue and regex issue
</commit_message>
<xml_diff>
--- a/Schedules/CM_course_schedule.xlsx
+++ b/Schedules/CM_course_schedule.xlsx
@@ -66,16 +66,16 @@
   </si>
   <si>
     <t>5
-CM-320-05815-nan-EAX-015
-CM-320-05815-nan-EAX-016</t>
+CM-320-05815-TBD-EAX-015
+CM-320-05815-TBD-EAX-016</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
     <t>9
-CSM-305-09814-nan-EAX-015
-CSM-305-09814-nan-EAX-016</t>
+CSM-305-09814-TBD-EAX-015
+CSM-305-09814-TBD-EAX-016</t>
   </si>
   <si>
     <t>11
@@ -102,8 +102,8 @@
   <si>
     <t>13
 CSM-225-13810-Trottier-EAX-017
-CSM-199-13805-nan-EAX-015
-CSM-199-13805-nan-EAX-016</t>
+CSM-199-13805-TBD-EAX-015
+CSM-199-13805-TBD-EAX-016</t>
   </si>
   <si>
     <t>14
@@ -162,8 +162,8 @@
   </si>
   <si>
     <t>11
-CSM-199-11810-nan-EAX-015
-CSM-199-11810-nan-EAX-016</t>
+CSM-199-11810-TBD-EAX-015
+CSM-199-11810-TBD-EAX-016</t>
   </si>
   <si>
     <t>21

</xml_diff>